<commit_message>
update add B1 B2
</commit_message>
<xml_diff>
--- a/DjLenna/evidence.xlsx
+++ b/DjLenna/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>98295FA7856DD91C175D37E25553960E8056431BC4826800A45FFDD30E8860EE</t>
+  </si>
+  <si>
+    <t>570B705D160750584DA835994DDF571EAD3AE0C4097ECB9EEDF5580D8D368DF1</t>
+  </si>
+  <si>
+    <t>71F818C97DC51D996A7E05BD94386D13CED1D151AF8ED9548A71DDD5A5B057B0</t>
+  </si>
+  <si>
+    <t>A92CB99055EC53E39B31BE2BA5FFFD5C195139215545ED331C4AA654B15AC99E</t>
+  </si>
+  <si>
+    <t>F6C8D6571A01384D3D0A012108AB05D589B394D546CAA5CE557B4F25F3D5815A</t>
   </si>
 </sst>
 </file>
@@ -3123,7 +3135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3595,7 +3607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3614,7 +3628,7 @@
     </row>
     <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3623,7 +3637,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3693,7 +3707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3712,7 +3728,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3721,7 +3737,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>

</xml_diff>